<commit_message>
chat retunring PL, next need to send it to AI... also enforce dates
</commit_message>
<xml_diff>
--- a/uploaded_files/cleaned_default_filename.xlsx
+++ b/uploaded_files/cleaned_default_filename.xlsx
@@ -441,62 +441,62 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Jan 2023</t>
+          <t>Oct 2023</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Feb 2023</t>
+          <t>Nov 2023</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Mar 2023</t>
+          <t>Dec 2023</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Apr 2023</t>
+          <t>Jan 2024</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>May 2023</t>
+          <t>Feb 2024</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Jun 2023</t>
+          <t>Mar 2024</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Jul 2023</t>
+          <t>Apr 2024</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Aug 2023</t>
+          <t>May 2024</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Sep 2023</t>
+          <t>Jun 2024</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Oct 2023</t>
+          <t>Jul 2024</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Nov 2023</t>
+          <t>Aug 2024</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Dec 2023</t>
+          <t>Sep 2024</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -520,13 +520,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>3250</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1125</v>
       </c>
       <c r="E2" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -547,10 +547,10 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>3250</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>1125</v>
+        <v>0</v>
       </c>
       <c r="N2" t="b">
         <v>0</v>
@@ -568,40 +568,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>3213.75</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1412.5</v>
       </c>
       <c r="D3" t="n">
-        <v>-5000</v>
+        <v>10542.36</v>
       </c>
       <c r="E3" t="n">
-        <v>21462.29</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1962.5</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>-988.5</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>7475</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>4299.8</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>3213.75</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>1412.5</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>10542.36</v>
+        <v>0</v>
       </c>
       <c r="N3" t="b">
         <v>0</v>
@@ -625,13 +625,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>33.33</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>33.33</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>33.33</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -640,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>99.98999999999999</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -670,40 +670,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1589.76</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>-537.8200000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>-7568.52</v>
+        <v>8068.03</v>
       </c>
       <c r="E5" t="n">
-        <v>19792.16</v>
+        <v>-1622.41</v>
       </c>
       <c r="F5" t="n">
-        <v>-1633.89</v>
+        <v>-1349.99</v>
       </c>
       <c r="G5" t="n">
-        <v>-436.07</v>
+        <v>-3015</v>
       </c>
       <c r="H5" t="n">
-        <v>-4298.15</v>
+        <v>-95</v>
       </c>
       <c r="I5" t="n">
-        <v>5699</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>1905.01</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>1589.76</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>-537.8200000000001</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>8068.03</v>
+        <v>0</v>
       </c>
       <c r="N5" t="b">
         <v>0</v>

</xml_diff>